<commit_message>
📊 Weekly driver report update for 2025-04-19
</commit_message>
<xml_diff>
--- a/Output/roaming_impact_reports_per_acct/AMD_driver_summary.xlsx
+++ b/Output/roaming_impact_reports_per_acct/AMD_driver_summary.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,161 +483,159 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.220.1.1</t>
+          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.18.2</t>
         </is>
       </c>
       <c r="B3" s="4" t="n">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>28863</v>
+        <v>1030</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>97.90000000000001</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 7265 - 19.51.18.1</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.220.1.1</t>
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>581</v>
+        <v>9599</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>97.90000000000001</v>
+        <v>98.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 22.110.1.1</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 21.60.0.5</t>
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>1453</v>
+        <v>1309</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>98.09999999999999</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.18.2</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.140.0.3</t>
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>2594</v>
+        <v>2</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>98.59999999999999</v>
+        <v>98.8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 22.160.0.3</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>98.8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 21.50.1.1</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>98.90000000000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Totals:</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n">
-        <v>72</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>33491</v>
-      </c>
-    </row>
-    <row r="8"/>
-    <row r="9"/>
+      <c r="B9" s="5" t="n">
+        <v>127</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>11988</v>
+      </c>
+    </row>
     <row r="10"/>
     <row r="11"/>
     <row r="12"/>
-    <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
         <is>
           <t>Good Drivers (Roaming &gt; 99.8%)</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>Adapter-Driver</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B16" s="3" t="inlineStr">
         <is>
           <t>Total Samples</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr"/>
-      <c r="D14" s="3" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr"/>
+      <c r="D16" s="3" t="inlineStr">
         <is>
           <t>Good Roaming Calculation (%)</t>
         </is>
       </c>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="E16" s="3" t="inlineStr">
         <is>
           <t>Driver Vintage</t>
         </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.50.0.5</t>
-        </is>
-      </c>
-      <c r="B15" s="6" t="n">
-        <v>269022</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" s="4" t="n">
-        <v>99.90000000000001</v>
-      </c>
-      <c r="E15" s="4" t="n">
-        <v/>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Intel(R) Dual Band Wireless-AC 7265 - 19.50.1.6</t>
-        </is>
-      </c>
-      <c r="B16" s="6" t="n">
-        <v>29259</v>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" s="4" t="n">
-        <v>99.90000000000001</v>
-      </c>
-      <c r="E16" s="4" t="n">
-        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 7265 - 19.51.8.3</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.160.0.4</t>
         </is>
       </c>
       <c r="B17" s="6" t="n">
-        <v>13028</v>
+        <v>96526</v>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" s="4" t="n">
-        <v>100</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="E17" s="4" t="n">
         <v/>
@@ -646,258 +644,236 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 23.100.0.4</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.230.0.8</t>
         </is>
       </c>
       <c r="B18" s="6" t="n">
-        <v>392601</v>
+        <v>328411</v>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" s="4" t="n">
         <v>99.90000000000001</v>
       </c>
-      <c r="E18" s="4" t="inlineStr">
-        <is>
-          <t>2024-11-10</t>
-        </is>
+      <c r="E18" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 7265 - 19.51.50.2</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.200.0.6</t>
         </is>
       </c>
       <c r="B19" s="6" t="n">
-        <v>19910</v>
+        <v>143808</v>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E19" s="4" t="inlineStr">
-        <is>
-          <t>2023-11-06</t>
-        </is>
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.150.3.1</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.190.0.4</t>
         </is>
       </c>
       <c r="B20" s="6" t="n">
-        <v>10661</v>
+        <v>287148</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E20" s="4" t="inlineStr">
-        <is>
-          <t>2022-08-29</t>
-        </is>
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E20" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.150.0.3</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.250.10.1</t>
         </is>
       </c>
       <c r="B21" s="6" t="n">
-        <v>14239</v>
+        <v>69578</v>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" s="4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E21" s="4" t="inlineStr">
-        <is>
-          <t>2022-05-23</t>
-        </is>
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E21" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.100.1.1</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.150.3.1</t>
         </is>
       </c>
       <c r="B22" s="6" t="n">
-        <v>254702</v>
+        <v>10661</v>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" s="4" t="n">
-        <v>99.90000000000001</v>
-      </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>2022-05-01</t>
-        </is>
+        <v>100</v>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 8260 - 22.80.1.1</t>
+          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 21.60.2.1</t>
         </is>
       </c>
       <c r="B23" s="6" t="n">
-        <v>117934</v>
+        <v>56018</v>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E23" s="4" t="inlineStr">
-        <is>
-          <t>2021-09-11</t>
-        </is>
+      <c r="E23" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.27.1</t>
+          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 22.50.1.1</t>
         </is>
       </c>
       <c r="B24" s="6" t="n">
-        <v>16089</v>
+        <v>34244</v>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E24" s="4" t="inlineStr">
-        <is>
-          <t>2021-09-11</t>
-        </is>
+      <c r="E24" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 22.80.0.9</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.30.0.11</t>
         </is>
       </c>
       <c r="B25" s="6" t="n">
-        <v>74604</v>
+        <v>67111</v>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" s="4" t="n">
-        <v>99.90000000000001</v>
-      </c>
-      <c r="E25" s="4" t="inlineStr">
-        <is>
-          <t>2021-08-18</t>
-        </is>
+        <v>100</v>
+      </c>
+      <c r="E25" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 22.50.1.1</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 21.30.4.1</t>
         </is>
       </c>
       <c r="B26" s="6" t="n">
-        <v>33050</v>
+        <v>13016</v>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E26" s="4" t="inlineStr">
-        <is>
-          <t>2021-04-27</t>
-        </is>
+      <c r="E26" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 21.110.3.2</t>
+          <t>Intel(R) Dual Band Wireless-AC 8260 - 22.180.0.4</t>
         </is>
       </c>
       <c r="B27" s="6" t="n">
-        <v>59673</v>
+        <v>10456</v>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E27" s="4" t="inlineStr">
-        <is>
-          <t>2020-08-05</t>
-        </is>
+      <c r="E27" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 7265 - 19.51.30.1</t>
+          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.50.0.5</t>
         </is>
       </c>
       <c r="B28" s="6" t="n">
-        <v>179007</v>
+        <v>288399</v>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="4" t="inlineStr">
-        <is>
-          <t>2020-06-01</t>
-        </is>
+      <c r="E28" s="4" t="n">
+        <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 7265 - 19.51.29.1</t>
+          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 23.100.0.4</t>
         </is>
       </c>
       <c r="B29" s="6" t="n">
-        <v>39767</v>
+        <v>442178</v>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" s="4" t="n">
-        <v>100</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="E29" s="4" t="inlineStr">
         <is>
-          <t>2020-04-15</t>
+          <t>2024-11-10</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 21.70.0.6</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 23.70.2.3</t>
         </is>
       </c>
       <c r="B30" s="6" t="n">
-        <v>107862</v>
+        <v>18721</v>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" s="4" t="n">
-        <v>100</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="E30" s="4" t="inlineStr">
         <is>
-          <t>2020-01-06</t>
+          <t>2024-07-23</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.16.4</t>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.10.0.7</t>
         </is>
       </c>
       <c r="B31" s="6" t="n">
-        <v>35023</v>
+        <v>66577</v>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" s="4" t="n">
@@ -905,18 +881,18 @@
       </c>
       <c r="E31" s="4" t="inlineStr">
         <is>
-          <t>2019-12-31</t>
+          <t>2024-05-09</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 21.60.2.1</t>
+          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.27.1</t>
         </is>
       </c>
       <c r="B32" s="6" t="n">
-        <v>56018</v>
+        <v>17529</v>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" s="4" t="n">
@@ -924,37 +900,37 @@
       </c>
       <c r="E32" s="4" t="inlineStr">
         <is>
-          <t>2019-12-14</t>
+          <t>2023-09-13</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.12.5</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.150.0.3</t>
         </is>
       </c>
       <c r="B33" s="6" t="n">
-        <v>173128</v>
+        <v>14239</v>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" s="4" t="n">
-        <v>99.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="E33" s="4" t="inlineStr">
         <is>
-          <t>2019-08-25</t>
+          <t>2022-05-23</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.5.2</t>
+          <t>Intel(R) Wi-Fi 6E AX211 160MHz - 22.100.1.1</t>
         </is>
       </c>
       <c r="B34" s="6" t="n">
-        <v>127188</v>
+        <v>265400</v>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" s="4" t="n">
@@ -962,18 +938,18 @@
       </c>
       <c r="E34" s="4" t="inlineStr">
         <is>
-          <t>2018-11-25</t>
+          <t>2022-05-01</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Intel(R) Dual Band Wireless-AC 7265 - 19.51.14.1</t>
+          <t>Intel(R) Dual Band Wireless-AC 8260 - 22.80.1.1</t>
         </is>
       </c>
       <c r="B35" s="6" t="n">
-        <v>112242</v>
+        <v>123675</v>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" s="4" t="n">
@@ -981,15 +957,205 @@
       </c>
       <c r="E35" s="4" t="inlineStr">
         <is>
-          <t>2018-05-26</t>
-        </is>
-      </c>
-    </row>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
+          <t>2021-09-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 22.80.0.9</t>
+        </is>
+      </c>
+      <c r="B36" s="6" t="n">
+        <v>77849</v>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" s="4" t="n">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E36" s="4" t="inlineStr">
+        <is>
+          <t>2021-08-18</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 21.60.2.1</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="n">
+        <v>26241</v>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E37" s="4" t="inlineStr">
+        <is>
+          <t>2021-01-19</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 22.0.1.1</t>
+        </is>
+      </c>
+      <c r="B38" s="6" t="n">
+        <v>15730</v>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" s="4" t="n">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E38" s="4" t="inlineStr">
+        <is>
+          <t>2020-09-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 21.110.3.2</t>
+        </is>
+      </c>
+      <c r="B39" s="6" t="n">
+        <v>59673</v>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E39" s="4" t="inlineStr">
+        <is>
+          <t>2020-08-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX201 160MHz - 21.70.0.6</t>
+        </is>
+      </c>
+      <c r="B40" s="6" t="n">
+        <v>113652</v>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E40" s="4" t="inlineStr">
+        <is>
+          <t>2019-12-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 21.40.2.2</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="n">
+        <v>88435</v>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" s="4" t="n">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E41" s="4" t="inlineStr">
+        <is>
+          <t>2019-08-31</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.12.5</t>
+        </is>
+      </c>
+      <c r="B42" s="6" t="n">
+        <v>180575</v>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" s="4" t="n">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E42" s="4" t="inlineStr">
+        <is>
+          <t>2019-08-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Intel(R) Wi-Fi 6 AX200 160MHz - 21.10.1.2</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="n">
+        <v>46270</v>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E43" s="4" t="inlineStr">
+        <is>
+          <t>2019-04-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.5.2</t>
+        </is>
+      </c>
+      <c r="B44" s="6" t="n">
+        <v>138724</v>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" s="4" t="n">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="E44" s="4" t="inlineStr">
+        <is>
+          <t>2018-11-25</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Intel(R) Dual Band Wireless-AC 8260 - 20.70.16.4</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="n">
+        <v>35023</v>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" s="4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>2018-03-26</t>
+        </is>
+      </c>
+    </row>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>